<commit_message>
Update indredients_database.xlsx and notes.txt
</commit_message>
<xml_diff>
--- a/IngredientConverterHelpers/ingredient_database.xlsx
+++ b/IngredientConverterHelpers/ingredient_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawndemeo/Development/Kitchen Converter App/IngredientConverterHelpers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19C620E-C5E3-5242-B854-95767362679F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC4DD8B-2968-DB44-8B59-D6839FEF52CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11500" yWindow="620" windowWidth="39700" windowHeight="26840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52200" yWindow="820" windowWidth="39700" windowHeight="26840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Butter</t>
   </si>
   <si>
-    <t>Fat</t>
-  </si>
-  <si>
     <t>stick</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t>Chopped chocolate</t>
   </si>
   <si>
-    <t>Nut</t>
-  </si>
-  <si>
     <t>Walnut halves</t>
   </si>
   <si>
@@ -235,9 +229,6 @@
     <t>White rice, uncooked</t>
   </si>
   <si>
-    <t>Grain</t>
-  </si>
-  <si>
     <t>Brown rice, uncooked</t>
   </si>
   <si>
@@ -250,12 +241,6 @@
     <t>Raisins</t>
   </si>
   <si>
-    <t>Dried Fruit</t>
-  </si>
-  <si>
-    <t>Vegetable</t>
-  </si>
-  <si>
     <t>clove</t>
   </si>
   <si>
@@ -289,9 +274,6 @@
     <t>Table salt</t>
   </si>
   <si>
-    <t>Spice</t>
-  </si>
-  <si>
     <t>Kosher salt</t>
   </si>
   <si>
@@ -307,9 +289,6 @@
     <t>Chili powder</t>
   </si>
   <si>
-    <t>Egg</t>
-  </si>
-  <si>
     <t>egg</t>
   </si>
   <si>
@@ -491,6 +470,42 @@
   </si>
   <si>
     <t>Graham crackers, crushed</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>Fats</t>
+  </si>
+  <si>
+    <t>Grains</t>
+  </si>
+  <si>
+    <t>Nuts</t>
+  </si>
+  <si>
+    <t>Spices</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Ketchup</t>
+  </si>
+  <si>
+    <t>Oyster sauce</t>
+  </si>
+  <si>
+    <t>Hoisin sauce</t>
+  </si>
+  <si>
+    <t>Mayonnaise</t>
+  </si>
+  <si>
+    <t>fdc.nal.usda.gov 10/19/2025</t>
+  </si>
+  <si>
+    <t>Sauces</t>
   </si>
 </sst>
 </file>
@@ -617,8 +632,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7623B37-8BEC-E14D-8697-159544536B92}" name="Table1" displayName="Table1" ref="A1:M115" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:M115" xr:uid="{A7623B37-8BEC-E14D-8697-159544536B92}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7623B37-8BEC-E14D-8697-159544536B92}" name="Table1" displayName="Table1" ref="A1:M121" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:M121" xr:uid="{A7623B37-8BEC-E14D-8697-159544536B92}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M115">
     <sortCondition ref="B2:B115"/>
     <sortCondition ref="A2:A115"/>
@@ -927,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M115"/>
+  <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -993,10 +1008,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1011,18 +1026,18 @@
         <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1037,18 +1052,18 @@
         <v>16</v>
       </c>
       <c r="L3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1063,18 +1078,18 @@
         <v>16</v>
       </c>
       <c r="L4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1089,18 +1104,18 @@
         <v>16</v>
       </c>
       <c r="L5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1115,18 +1130,18 @@
         <v>16</v>
       </c>
       <c r="L6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1141,18 +1156,18 @@
         <v>16</v>
       </c>
       <c r="L7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1167,18 +1182,18 @@
         <v>16</v>
       </c>
       <c r="L8" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1193,18 +1208,18 @@
         <v>16</v>
       </c>
       <c r="L9" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M9" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1219,18 +1234,18 @@
         <v>16</v>
       </c>
       <c r="L10" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
         <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1245,18 +1260,18 @@
         <v>16</v>
       </c>
       <c r="L11" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
         <v>60</v>
-      </c>
-      <c r="B12" t="s">
-        <v>61</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1271,18 +1286,18 @@
         <v>16</v>
       </c>
       <c r="L12" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1297,18 +1312,18 @@
         <v>16</v>
       </c>
       <c r="L13" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M13" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1320,21 +1335,21 @@
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="L14" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M14" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1349,18 +1364,18 @@
         <v>16</v>
       </c>
       <c r="L15" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M15" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1375,18 +1390,18 @@
         <v>16</v>
       </c>
       <c r="L16" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M16" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1401,18 +1416,18 @@
         <v>16</v>
       </c>
       <c r="L17" t="s">
+        <v>100</v>
+      </c>
+      <c r="M17" t="s">
         <v>107</v>
-      </c>
-      <c r="M17" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1427,18 +1442,18 @@
         <v>16</v>
       </c>
       <c r="L18" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M18" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1453,18 +1468,18 @@
         <v>16</v>
       </c>
       <c r="L19" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M19" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1479,18 +1494,18 @@
         <v>16</v>
       </c>
       <c r="L20" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M20" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1505,18 +1520,18 @@
         <v>16</v>
       </c>
       <c r="L21" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M21" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1531,18 +1546,18 @@
         <v>16</v>
       </c>
       <c r="L22" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M22" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1557,18 +1572,18 @@
         <v>16</v>
       </c>
       <c r="L23" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M23" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
         <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>44</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1583,18 +1598,18 @@
         <v>16</v>
       </c>
       <c r="L24" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M24" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
         <v>43</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1609,296 +1624,299 @@
         <v>16</v>
       </c>
       <c r="L25" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M25" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>15</v>
+      <c r="F26" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" t="s">
+        <v>92</v>
       </c>
       <c r="H26">
-        <v>130</v>
+        <v>33</v>
       </c>
       <c r="I26" t="s">
         <v>16</v>
       </c>
       <c r="L26" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M26" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" t="s">
-        <v>15</v>
+      <c r="F27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" t="s">
+        <v>94</v>
       </c>
       <c r="H27">
-        <v>160</v>
+        <v>17</v>
       </c>
       <c r="I27" t="s">
         <v>16</v>
       </c>
       <c r="L27" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M27" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28" t="s">
-        <v>15</v>
+      <c r="F28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" t="s">
+        <v>90</v>
       </c>
       <c r="H28">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="I28" t="s">
         <v>16</v>
       </c>
       <c r="L28" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M28" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
-        <v>15</v>
+      <c r="F29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" t="s">
+        <v>90</v>
       </c>
       <c r="H29">
-        <v>165</v>
+        <v>50</v>
       </c>
       <c r="I29" t="s">
         <v>16</v>
       </c>
       <c r="L29" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M29" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="G30" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="H30">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="I30" t="s">
         <v>16</v>
       </c>
       <c r="L30" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M30" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G31" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="H31">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="I31" t="s">
         <v>16</v>
       </c>
       <c r="L31" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M31" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="F32" t="s">
-        <v>96</v>
-      </c>
-      <c r="G32" t="s">
-        <v>97</v>
+      <c r="E32" t="s">
+        <v>15</v>
       </c>
       <c r="H32">
-        <v>56</v>
+        <v>227</v>
       </c>
       <c r="I32" t="s">
         <v>16</v>
       </c>
       <c r="L32" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M32" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="F33" t="s">
-        <v>96</v>
-      </c>
-      <c r="G33" t="s">
-        <v>97</v>
+      <c r="E33" t="s">
+        <v>17</v>
       </c>
       <c r="H33">
-        <v>50</v>
+        <v>14.2</v>
       </c>
       <c r="I33" t="s">
         <v>16</v>
       </c>
       <c r="L33" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M33" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="F34" t="s">
-        <v>96</v>
-      </c>
-      <c r="G34" t="s">
-        <v>97</v>
+      <c r="E34" t="s">
+        <v>28</v>
       </c>
       <c r="H34">
-        <v>57</v>
+        <v>4.7</v>
       </c>
       <c r="I34" t="s">
         <v>16</v>
       </c>
       <c r="L34" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M34" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>151</v>
       </c>
-      <c r="B35" t="s">
-        <v>95</v>
-      </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="G35" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="H35">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="I35" t="s">
         <v>16</v>
       </c>
       <c r="L35" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M35" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1907,97 +1925,94 @@
         <v>15</v>
       </c>
       <c r="H36">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="I36" t="s">
         <v>16</v>
       </c>
       <c r="L36" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M36" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H37">
-        <v>14.2</v>
+        <v>205</v>
       </c>
       <c r="I37" t="s">
         <v>16</v>
       </c>
       <c r="L37" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M37" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H38">
-        <v>4.7</v>
+        <v>216</v>
       </c>
       <c r="I38" t="s">
         <v>16</v>
       </c>
       <c r="L38" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M38" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="F39" t="s">
-        <v>36</v>
-      </c>
-      <c r="G39" t="s">
-        <v>37</v>
+      <c r="E39" t="s">
+        <v>17</v>
       </c>
       <c r="H39">
-        <v>113</v>
+        <v>13.5</v>
       </c>
       <c r="I39" t="s">
         <v>16</v>
       </c>
       <c r="L39" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M39" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -2005,7 +2020,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -2014,24 +2029,24 @@
         <v>15</v>
       </c>
       <c r="H40">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="I40" t="s">
         <v>16</v>
       </c>
       <c r="L40" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M40" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2040,102 +2055,102 @@
         <v>15</v>
       </c>
       <c r="H41">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="I41" t="s">
         <v>16</v>
       </c>
       <c r="L41" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M41" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H42">
-        <v>216</v>
+        <v>13.6</v>
       </c>
       <c r="I42" t="s">
         <v>16</v>
       </c>
       <c r="L42" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M42" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H43">
-        <v>13.5</v>
+        <v>120</v>
       </c>
       <c r="I43" t="s">
         <v>16</v>
       </c>
       <c r="L43" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M43" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H44">
-        <v>205</v>
+        <v>7.5</v>
       </c>
       <c r="I44" t="s">
         <v>16</v>
       </c>
       <c r="L44" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M44" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2144,47 +2159,47 @@
         <v>15</v>
       </c>
       <c r="H45">
-        <v>218</v>
+        <v>96</v>
       </c>
       <c r="I45" t="s">
         <v>16</v>
       </c>
       <c r="L45" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M45" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H46">
-        <v>13.6</v>
+        <v>120</v>
       </c>
       <c r="I46" t="s">
         <v>16</v>
       </c>
       <c r="L46" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M46" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
         <v>14</v>
@@ -2202,15 +2217,15 @@
         <v>16</v>
       </c>
       <c r="L47" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M47" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B48" t="s">
         <v>14</v>
@@ -2219,24 +2234,24 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H48">
-        <v>7.5</v>
+        <v>128</v>
       </c>
       <c r="I48" t="s">
         <v>16</v>
       </c>
       <c r="L48" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M48" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
         <v>14</v>
@@ -2248,21 +2263,21 @@
         <v>15</v>
       </c>
       <c r="H49">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I49" t="s">
         <v>16</v>
       </c>
       <c r="L49" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M49" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
         <v>14</v>
@@ -2274,21 +2289,21 @@
         <v>15</v>
       </c>
       <c r="H50">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="I50" t="s">
         <v>16</v>
       </c>
       <c r="L50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M50" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
@@ -2300,21 +2315,21 @@
         <v>15</v>
       </c>
       <c r="H51">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I51" t="s">
         <v>16</v>
       </c>
       <c r="L51" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M51" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
         <v>14</v>
@@ -2326,50 +2341,53 @@
         <v>15</v>
       </c>
       <c r="H52">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="I52" t="s">
         <v>16</v>
       </c>
       <c r="L52" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M52" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>136</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
-      <c r="E53" t="s">
-        <v>15</v>
+      <c r="F53" t="s">
+        <v>76</v>
+      </c>
+      <c r="G53" t="s">
+        <v>77</v>
       </c>
       <c r="H53">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="I53" t="s">
         <v>16</v>
       </c>
       <c r="L53" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M53" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -2378,50 +2396,53 @@
         <v>15</v>
       </c>
       <c r="H54">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="I54" t="s">
         <v>16</v>
       </c>
       <c r="L54" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M54" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>137</v>
       </c>
       <c r="B55" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
-      <c r="E55" t="s">
-        <v>15</v>
+      <c r="F55" t="s">
+        <v>78</v>
+      </c>
+      <c r="G55" t="s">
+        <v>79</v>
       </c>
       <c r="H55">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="I55" t="s">
         <v>16</v>
       </c>
       <c r="L55" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M55" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -2430,137 +2451,131 @@
         <v>15</v>
       </c>
       <c r="H56">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="I56" t="s">
         <v>16</v>
       </c>
       <c r="L56" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M56" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
-      <c r="F57" t="s">
-        <v>81</v>
-      </c>
-      <c r="G57" t="s">
-        <v>82</v>
+      <c r="E57" t="s">
+        <v>15</v>
       </c>
       <c r="H57">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="I57" t="s">
         <v>16</v>
       </c>
       <c r="L57" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M57" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
-      <c r="F58" t="s">
-        <v>83</v>
-      </c>
-      <c r="G58" t="s">
-        <v>84</v>
+      <c r="E58" t="s">
+        <v>15</v>
       </c>
       <c r="H58">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="I58" t="s">
         <v>16</v>
       </c>
       <c r="L58" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M58" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="B59" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
         <v>80</v>
       </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59" t="s">
-        <v>15</v>
+      <c r="G59" t="s">
+        <v>81</v>
       </c>
       <c r="H59">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="I59" t="s">
         <v>16</v>
       </c>
       <c r="L59" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M59" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
-      <c r="F60" t="s">
-        <v>85</v>
-      </c>
-      <c r="G60" t="s">
-        <v>86</v>
+      <c r="E60" t="s">
+        <v>15</v>
       </c>
       <c r="H60">
-        <v>58</v>
+        <v>165</v>
       </c>
       <c r="I60" t="s">
         <v>16</v>
       </c>
       <c r="L60" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M60" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B61" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -2575,18 +2590,18 @@
         <v>16</v>
       </c>
       <c r="L61" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M61" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -2601,18 +2616,18 @@
         <v>16</v>
       </c>
       <c r="L62" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M62" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2627,18 +2642,18 @@
         <v>16</v>
       </c>
       <c r="L63" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M63" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -2653,18 +2668,18 @@
         <v>16</v>
       </c>
       <c r="L64" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M64" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -2679,18 +2694,18 @@
         <v>16</v>
       </c>
       <c r="L65" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M65" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -2705,18 +2720,18 @@
         <v>16</v>
       </c>
       <c r="L66" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M66" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -2731,18 +2746,18 @@
         <v>16</v>
       </c>
       <c r="L67" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M67" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -2757,18 +2772,18 @@
         <v>16</v>
       </c>
       <c r="L68" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M68" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B69" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -2783,18 +2798,18 @@
         <v>16</v>
       </c>
       <c r="L69" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M69" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B70" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -2809,18 +2824,18 @@
         <v>16</v>
       </c>
       <c r="L70" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M70" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -2835,18 +2850,18 @@
         <v>16</v>
       </c>
       <c r="L71" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M71" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B72" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -2861,18 +2876,18 @@
         <v>16</v>
       </c>
       <c r="L72" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M72" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -2887,18 +2902,18 @@
         <v>16</v>
       </c>
       <c r="L73" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M73" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B74" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -2913,18 +2928,18 @@
         <v>16</v>
       </c>
       <c r="L74" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M74" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B75" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -2939,18 +2954,18 @@
         <v>16</v>
       </c>
       <c r="L75" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M75" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -2965,18 +2980,18 @@
         <v>16</v>
       </c>
       <c r="L76" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M76" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B77" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -2991,18 +3006,18 @@
         <v>16</v>
       </c>
       <c r="L77" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M77" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B78" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -3017,27 +3032,27 @@
         <v>16</v>
       </c>
       <c r="L78" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M78" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B79" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="G79" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H79">
         <v>15</v>
@@ -3046,18 +3061,18 @@
         <v>16</v>
       </c>
       <c r="L79" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M79" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B80" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -3072,18 +3087,18 @@
         <v>16</v>
       </c>
       <c r="L80" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M80" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B81" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -3098,18 +3113,18 @@
         <v>16</v>
       </c>
       <c r="L81" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M81" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B82" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -3124,18 +3139,18 @@
         <v>16</v>
       </c>
       <c r="L82" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M82" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B83" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -3150,18 +3165,18 @@
         <v>16</v>
       </c>
       <c r="L83" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M83" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B84" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -3176,18 +3191,18 @@
         <v>16</v>
       </c>
       <c r="L84" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M84" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B85" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -3202,18 +3217,18 @@
         <v>16</v>
       </c>
       <c r="L85" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M85" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -3228,18 +3243,18 @@
         <v>16</v>
       </c>
       <c r="L86" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M86" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B87" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -3254,21 +3269,21 @@
         <v>16</v>
       </c>
       <c r="L87" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M87" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B88" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="C88" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -3283,21 +3298,21 @@
         <v>16</v>
       </c>
       <c r="L88" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M88" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="C89" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -3312,18 +3327,18 @@
         <v>16</v>
       </c>
       <c r="L89" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M89" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -3338,18 +3353,18 @@
         <v>16</v>
       </c>
       <c r="L90" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M90" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B91" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -3364,18 +3379,18 @@
         <v>16</v>
       </c>
       <c r="L91" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M91" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B92" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -3390,10 +3405,10 @@
         <v>16</v>
       </c>
       <c r="L92" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M92" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
@@ -3416,10 +3431,10 @@
         <v>16</v>
       </c>
       <c r="L93" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M93" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
@@ -3442,10 +3457,10 @@
         <v>16</v>
       </c>
       <c r="L94" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M94" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
@@ -3468,10 +3483,10 @@
         <v>16</v>
       </c>
       <c r="L95" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M95" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -3494,10 +3509,10 @@
         <v>16</v>
       </c>
       <c r="L96" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M96" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
@@ -3520,10 +3535,10 @@
         <v>16</v>
       </c>
       <c r="L97" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M97" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
@@ -3546,10 +3561,10 @@
         <v>16</v>
       </c>
       <c r="L98" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M98" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
@@ -3572,10 +3587,10 @@
         <v>16</v>
       </c>
       <c r="L99" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M99" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
@@ -3598,10 +3613,10 @@
         <v>16</v>
       </c>
       <c r="L100" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M100" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
@@ -3624,10 +3639,10 @@
         <v>16</v>
       </c>
       <c r="L101" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M101" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
@@ -3650,10 +3665,10 @@
         <v>16</v>
       </c>
       <c r="L102" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M102" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -3676,10 +3691,10 @@
         <v>16</v>
       </c>
       <c r="L103" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M103" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -3702,15 +3717,15 @@
         <v>16</v>
       </c>
       <c r="L104" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M104" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B105" t="s">
         <v>27</v>
@@ -3728,15 +3743,15 @@
         <v>16</v>
       </c>
       <c r="L105" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M105" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
         <v>27</v>
@@ -3754,18 +3769,18 @@
         <v>16</v>
       </c>
       <c r="L106" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M106" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B107" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -3780,27 +3795,27 @@
         <v>16</v>
       </c>
       <c r="L107" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M107" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B108" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D108">
         <v>1</v>
       </c>
       <c r="F108" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G108" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H108">
         <v>3</v>
@@ -3809,18 +3824,18 @@
         <v>16</v>
       </c>
       <c r="L108" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M108" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B109" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -3835,18 +3850,18 @@
         <v>16</v>
       </c>
       <c r="L109" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M109" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B110" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -3861,18 +3876,18 @@
         <v>16</v>
       </c>
       <c r="L110" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M110" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B111" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -3887,18 +3902,18 @@
         <v>16</v>
       </c>
       <c r="L111" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M111" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B112" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D112">
         <v>1</v>
@@ -3913,18 +3928,18 @@
         <v>16</v>
       </c>
       <c r="L112" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M112" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B113" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -3939,18 +3954,18 @@
         <v>16</v>
       </c>
       <c r="L113" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M113" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B114" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -3965,18 +3980,18 @@
         <v>16</v>
       </c>
       <c r="L114" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M114" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B115" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -3991,10 +4006,166 @@
         <v>16</v>
       </c>
       <c r="L115" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M115" t="s">
-        <v>117</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>156</v>
+      </c>
+      <c r="B116" t="s">
+        <v>96</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116" t="s">
+        <v>17</v>
+      </c>
+      <c r="H116">
+        <v>17</v>
+      </c>
+      <c r="I116" t="s">
+        <v>16</v>
+      </c>
+      <c r="L116" t="s">
+        <v>100</v>
+      </c>
+      <c r="M116" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>156</v>
+      </c>
+      <c r="B117" t="s">
+        <v>96</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117" t="s">
+        <v>15</v>
+      </c>
+      <c r="H117">
+        <v>240</v>
+      </c>
+      <c r="I117" t="s">
+        <v>16</v>
+      </c>
+      <c r="L117" t="s">
+        <v>100</v>
+      </c>
+      <c r="M117" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>157</v>
+      </c>
+      <c r="B118" t="s">
+        <v>161</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118" t="s">
+        <v>17</v>
+      </c>
+      <c r="H118">
+        <v>18</v>
+      </c>
+      <c r="I118" t="s">
+        <v>16</v>
+      </c>
+      <c r="L118" t="s">
+        <v>100</v>
+      </c>
+      <c r="M118" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>158</v>
+      </c>
+      <c r="B119" t="s">
+        <v>161</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119" t="s">
+        <v>17</v>
+      </c>
+      <c r="H119">
+        <v>16</v>
+      </c>
+      <c r="I119" t="s">
+        <v>16</v>
+      </c>
+      <c r="L119" t="s">
+        <v>100</v>
+      </c>
+      <c r="M119" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>159</v>
+      </c>
+      <c r="B120" t="s">
+        <v>151</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120" t="s">
+        <v>17</v>
+      </c>
+      <c r="H120">
+        <v>13.8</v>
+      </c>
+      <c r="I120" t="s">
+        <v>16</v>
+      </c>
+      <c r="L120" t="s">
+        <v>100</v>
+      </c>
+      <c r="M120" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>159</v>
+      </c>
+      <c r="B121" t="s">
+        <v>151</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121" t="s">
+        <v>15</v>
+      </c>
+      <c r="H121">
+        <v>220</v>
+      </c>
+      <c r="I121" t="s">
+        <v>16</v>
+      </c>
+      <c r="L121" t="s">
+        <v>100</v>
+      </c>
+      <c r="M121" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new ingredients to default database
- Add sliced mushrooms
- Add nonfat dried milk
</commit_message>
<xml_diff>
--- a/IngredientConverterHelpers/ingredient_database.xlsx
+++ b/IngredientConverterHelpers/ingredient_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawndemeo/Development/Kitchen Converter App/IngredientConverterHelpers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A970D2-C9DE-914B-B739-853F7147684D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DDCE6C-A185-844F-8DCD-13FCCBA16A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52240" yWindow="620" windowWidth="39700" windowHeight="26840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52240" yWindow="620" windowWidth="37880" windowHeight="26840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="289">
   <si>
     <t>Name</t>
   </si>
@@ -472,9 +472,6 @@
     <t>Ground ginger</t>
   </si>
   <si>
-    <t>Brown sugar</t>
-  </si>
-  <si>
     <t>Garlic clove</t>
   </si>
   <si>
@@ -869,6 +866,27 @@
   </si>
   <si>
     <t>0f49a639-b188-46c1-9b93-75b6715d2717</t>
+  </si>
+  <si>
+    <t>Brown sugar, packed</t>
+  </si>
+  <si>
+    <t>Semolina</t>
+  </si>
+  <si>
+    <t>fdc.nal.usda.gov 10/28/2025</t>
+  </si>
+  <si>
+    <t>Nonfat dried milk</t>
+  </si>
+  <si>
+    <t>King Arthur 10/28/2025</t>
+  </si>
+  <si>
+    <t>ae2f976d-b43e-4c3e-8f49-4682a99548ec</t>
+  </si>
+  <si>
+    <t>2923bebb-2e9e-46d1-8738-d6109def788a</t>
   </si>
 </sst>
 </file>
@@ -1036,8 +1054,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7623B37-8BEC-E14D-8697-159544536B92}" name="Table1" displayName="Table1" ref="A1:N131" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
-  <autoFilter ref="A1:N131" xr:uid="{A7623B37-8BEC-E14D-8697-159544536B92}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7623B37-8BEC-E14D-8697-159544536B92}" name="Table1" displayName="Table1" ref="A1:N133" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+  <autoFilter ref="A1:N133" xr:uid="{A7623B37-8BEC-E14D-8697-159544536B92}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:N131">
     <sortCondition ref="C2:C115"/>
     <sortCondition ref="B2:B115"/>
@@ -1347,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N131"/>
+  <dimension ref="A1:N133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1374,7 +1392,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1418,7 +1436,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
@@ -1447,7 +1465,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
@@ -1476,7 +1494,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
         <v>52</v>
@@ -1505,7 +1523,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
         <v>54</v>
@@ -1534,7 +1552,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
         <v>56</v>
@@ -1563,7 +1581,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" t="s">
         <v>57</v>
@@ -1592,7 +1610,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
         <v>55</v>
@@ -1621,7 +1639,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
@@ -1650,7 +1668,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
@@ -1679,7 +1697,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
@@ -1708,7 +1726,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
         <v>58</v>
@@ -1737,13 +1755,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1761,18 +1779,18 @@
         <v>96</v>
       </c>
       <c r="N13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1790,18 +1808,18 @@
         <v>96</v>
       </c>
       <c r="N14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1819,18 +1837,18 @@
         <v>96</v>
       </c>
       <c r="N15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s">
         <v>119</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1853,13 +1871,13 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s">
         <v>117</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1882,13 +1900,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B18" t="s">
         <v>117</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1911,13 +1929,13 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B19" t="s">
         <v>118</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1940,13 +1958,13 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1964,18 +1982,18 @@
         <v>96</v>
       </c>
       <c r="N20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1993,18 +2011,18 @@
         <v>96</v>
       </c>
       <c r="N21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" t="s">
         <v>171</v>
-      </c>
-      <c r="C22" t="s">
-        <v>172</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -2022,12 +2040,12 @@
         <v>96</v>
       </c>
       <c r="N22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
@@ -2056,7 +2074,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
@@ -2085,7 +2103,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s">
         <v>48</v>
@@ -2114,7 +2132,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
@@ -2143,7 +2161,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B27" t="s">
         <v>43</v>
@@ -2172,7 +2190,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
         <v>43</v>
@@ -2201,7 +2219,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B29" t="s">
         <v>111</v>
@@ -2230,7 +2248,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s">
         <v>45</v>
@@ -2259,7 +2277,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B31" t="s">
         <v>49</v>
@@ -2288,7 +2306,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
         <v>122</v>
@@ -2317,7 +2335,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B33" t="s">
         <v>44</v>
@@ -2346,7 +2364,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B34" t="s">
         <v>41</v>
@@ -2375,7 +2393,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B35" t="s">
         <v>41</v>
@@ -2404,10 +2422,10 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C36" t="s">
         <v>112</v>
@@ -2431,12 +2449,12 @@
         <v>96</v>
       </c>
       <c r="N36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B37" t="s">
         <v>125</v>
@@ -2468,7 +2486,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B38" t="s">
         <v>123</v>
@@ -2500,7 +2518,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B39" t="s">
         <v>127</v>
@@ -2532,7 +2550,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B40" t="s">
         <v>124</v>
@@ -2564,7 +2582,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B41" t="s">
         <v>126</v>
@@ -2596,7 +2614,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B42" t="s">
         <v>128</v>
@@ -2628,7 +2646,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B43" t="s">
         <v>33</v>
@@ -2657,7 +2675,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B44" t="s">
         <v>33</v>
@@ -2686,7 +2704,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B45" t="s">
         <v>33</v>
@@ -2715,7 +2733,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B46" t="s">
         <v>33</v>
@@ -2747,7 +2765,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B47" t="s">
         <v>38</v>
@@ -2776,7 +2794,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B48" t="s">
         <v>40</v>
@@ -2805,7 +2823,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B49" t="s">
         <v>120</v>
@@ -2834,7 +2852,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B50" t="s">
         <v>120</v>
@@ -2863,7 +2881,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B51" t="s">
         <v>37</v>
@@ -2892,7 +2910,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B52" t="s">
         <v>37</v>
@@ -2921,7 +2939,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B53" t="s">
         <v>39</v>
@@ -2950,7 +2968,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B54" t="s">
         <v>36</v>
@@ -2979,7 +2997,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B55" t="s">
         <v>36</v>
@@ -3008,7 +3026,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B56" t="s">
         <v>13</v>
@@ -3037,7 +3055,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B57" t="s">
         <v>13</v>
@@ -3066,7 +3084,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B58" t="s">
         <v>22</v>
@@ -3095,7 +3113,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
@@ -3124,7 +3142,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B60" t="s">
         <v>19</v>
@@ -3153,7 +3171,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B61" t="s">
         <v>23</v>
@@ -3182,7 +3200,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B62" t="s">
         <v>25</v>
@@ -3211,7 +3229,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
@@ -3240,7 +3258,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B64" t="s">
         <v>21</v>
@@ -3269,7 +3287,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B65" t="s">
         <v>20</v>
@@ -3298,7 +3316,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B66" t="s">
         <v>78</v>
@@ -3327,7 +3345,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B67" t="s">
         <v>133</v>
@@ -3356,7 +3374,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B68" t="s">
         <v>129</v>
@@ -3385,7 +3403,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B69" t="s">
         <v>132</v>
@@ -3414,7 +3432,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B70" t="s">
         <v>130</v>
@@ -3446,7 +3464,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B71" t="s">
         <v>131</v>
@@ -3478,7 +3496,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B72" t="s">
         <v>134</v>
@@ -3510,7 +3528,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B73" t="s">
         <v>68</v>
@@ -3539,7 +3557,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B74" t="s">
         <v>135</v>
@@ -3568,7 +3586,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B75" t="s">
         <v>136</v>
@@ -3597,7 +3615,7 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B76" t="s">
         <v>137</v>
@@ -3626,7 +3644,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B77" t="s">
         <v>138</v>
@@ -3655,7 +3673,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B78" t="s">
         <v>67</v>
@@ -3684,7 +3702,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B79" t="s">
         <v>139</v>
@@ -3713,7 +3731,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B80" t="s">
         <v>140</v>
@@ -3742,7 +3760,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B81" t="s">
         <v>141</v>
@@ -3771,13 +3789,13 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B82" t="s">
         <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -3800,13 +3818,13 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C83" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E83">
         <v>2</v>
@@ -3824,18 +3842,18 @@
         <v>96</v>
       </c>
       <c r="N83" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B84" t="s">
         <v>110</v>
       </c>
       <c r="C84" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -3858,13 +3876,13 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B85" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C85" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E85">
         <v>0.25</v>
@@ -3882,18 +3900,18 @@
         <v>96</v>
       </c>
       <c r="N85" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B86" t="s">
         <v>82</v>
       </c>
       <c r="C86" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -3916,13 +3934,13 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B87" t="s">
         <v>147</v>
       </c>
       <c r="C87" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -3945,13 +3963,13 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B88" t="s">
         <v>148</v>
       </c>
       <c r="C88" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -3974,13 +3992,13 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B89" t="s">
         <v>149</v>
       </c>
       <c r="C89" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -4003,13 +4021,13 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B90" t="s">
         <v>80</v>
       </c>
       <c r="C90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D90" t="s">
         <v>108</v>
@@ -4035,13 +4053,13 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B91" t="s">
         <v>80</v>
       </c>
       <c r="C91" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D91" t="s">
         <v>109</v>
@@ -4067,13 +4085,13 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B92" t="s">
         <v>83</v>
       </c>
       <c r="C92" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -4096,13 +4114,13 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B93" t="s">
         <v>81</v>
       </c>
       <c r="C93" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -4125,13 +4143,13 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B94" t="s">
         <v>79</v>
       </c>
       <c r="C94" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -4154,7 +4172,7 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B95" t="s">
         <v>63</v>
@@ -4183,7 +4201,7 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B96" t="s">
         <v>144</v>
@@ -4212,7 +4230,7 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B97" t="s">
         <v>145</v>
@@ -4241,7 +4259,7 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B98" t="s">
         <v>65</v>
@@ -4270,7 +4288,7 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B99" t="s">
         <v>65</v>
@@ -4299,7 +4317,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B100" t="s">
         <v>64</v>
@@ -4328,7 +4346,7 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B101" t="s">
         <v>142</v>
@@ -4357,7 +4375,7 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B102" t="s">
         <v>66</v>
@@ -4386,7 +4404,7 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B103" t="s">
         <v>62</v>
@@ -4415,7 +4433,7 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B104" t="s">
         <v>143</v>
@@ -4444,7 +4462,7 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B105" t="s">
         <v>146</v>
@@ -4473,7 +4491,7 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B106" t="s">
         <v>93</v>
@@ -4505,10 +4523,10 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B107" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C107" t="s">
         <v>92</v>
@@ -4529,12 +4547,12 @@
         <v>96</v>
       </c>
       <c r="N107" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B108" t="s">
         <v>91</v>
@@ -4563,10 +4581,10 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B109" t="s">
-        <v>150</v>
+        <v>282</v>
       </c>
       <c r="C109" t="s">
         <v>27</v>
@@ -4592,10 +4610,10 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B110" t="s">
-        <v>150</v>
+        <v>282</v>
       </c>
       <c r="C110" t="s">
         <v>27</v>
@@ -4621,7 +4639,7 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B111" t="s">
         <v>31</v>
@@ -4650,7 +4668,7 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B112" t="s">
         <v>26</v>
@@ -4679,7 +4697,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B113" t="s">
         <v>26</v>
@@ -4708,7 +4726,7 @@
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B114" t="s">
         <v>26</v>
@@ -4737,7 +4755,7 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B115" t="s">
         <v>29</v>
@@ -4766,7 +4784,7 @@
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B116" t="s">
         <v>29</v>
@@ -4795,7 +4813,7 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B117" t="s">
         <v>30</v>
@@ -4824,7 +4842,7 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B118" t="s">
         <v>30</v>
@@ -4853,7 +4871,7 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B119" t="s">
         <v>32</v>
@@ -4882,7 +4900,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B120" t="s">
         <v>32</v>
@@ -4911,7 +4929,7 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B121" t="s">
         <v>101</v>
@@ -4940,7 +4958,7 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B122" t="s">
         <v>101</v>
@@ -4969,10 +4987,10 @@
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B123" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C123" t="s">
         <v>116</v>
@@ -4998,10 +5016,10 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B124" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C124" t="s">
         <v>116</v>
@@ -5027,10 +5045,10 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B125" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>116</v>
@@ -5056,10 +5074,10 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B126" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C126" t="s">
         <v>116</v>
@@ -5085,10 +5103,10 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B127" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C127" t="s">
         <v>116</v>
@@ -5114,10 +5132,10 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B128" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C128" t="s">
         <v>116</v>
@@ -5143,10 +5161,10 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B129" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C129" t="s">
         <v>116</v>
@@ -5175,10 +5193,10 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B130" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C130" t="s">
         <v>116</v>
@@ -5204,10 +5222,10 @@
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B131" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C131" t="s">
         <v>116</v>
@@ -5229,6 +5247,64 @@
       </c>
       <c r="N131" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>287</v>
+      </c>
+      <c r="B132" t="s">
+        <v>283</v>
+      </c>
+      <c r="C132" t="s">
+        <v>14</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132" t="s">
+        <v>15</v>
+      </c>
+      <c r="I132">
+        <v>167</v>
+      </c>
+      <c r="J132" t="s">
+        <v>16</v>
+      </c>
+      <c r="M132" t="s">
+        <v>96</v>
+      </c>
+      <c r="N132" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>288</v>
+      </c>
+      <c r="B133" t="s">
+        <v>285</v>
+      </c>
+      <c r="C133" t="s">
+        <v>42</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133" t="s">
+        <v>15</v>
+      </c>
+      <c r="I133">
+        <v>112</v>
+      </c>
+      <c r="J133" t="s">
+        <v>16</v>
+      </c>
+      <c r="M133" t="s">
+        <v>96</v>
+      </c>
+      <c r="N133" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>